<commit_message>
Fixed the list of column names and classes on worksheet #2.  (The first column name, 'site', was not present in that list.)
</commit_message>
<xml_diff>
--- a/ARDEC_Plant_CN_Template.xlsx
+++ b/ARDEC_Plant_CN_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="-45" windowWidth="25020" windowHeight="12810"/>
+    <workbookView xWindow="6315" yWindow="-45" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="56">
   <si>
     <t>site</t>
   </si>
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -223,6 +223,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,11 +251,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -271,6 +274,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma0" xfId="1"/>
@@ -575,16 +584,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W1" sqref="W1:X1"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11" style="2"/>
+    <col min="4" max="4" width="11" style="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="11" style="13"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
@@ -597,76 +607,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -680,7 +690,7 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>6</v>
       </c>
       <c r="E2" t="s">
@@ -695,7 +705,7 @@
       <c r="H2">
         <v>85</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="13" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
@@ -727,7 +737,7 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>6</v>
       </c>
       <c r="E3" t="s">
@@ -742,7 +752,7 @@
       <c r="H3">
         <v>85</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J3" t="s">
@@ -774,7 +784,7 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>6</v>
       </c>
       <c r="E4">
@@ -789,7 +799,7 @@
       <c r="H4">
         <v>85</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J4" t="s">
@@ -821,7 +831,7 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>6</v>
       </c>
       <c r="E5">
@@ -836,7 +846,7 @@
       <c r="H5">
         <v>85</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J5" t="s">
@@ -868,7 +878,7 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>6</v>
       </c>
       <c r="E6">
@@ -883,7 +893,7 @@
       <c r="H6">
         <v>85</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J6" t="s">
@@ -915,7 +925,7 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>6</v>
       </c>
       <c r="F7" t="s">
@@ -927,7 +937,7 @@
       <c r="H7">
         <v>86</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="13" t="s">
         <v>18</v>
       </c>
       <c r="J7" t="s">
@@ -959,7 +969,7 @@
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>6</v>
       </c>
       <c r="F8" t="s">
@@ -971,7 +981,7 @@
       <c r="H8">
         <v>86</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J8" t="s">
@@ -1003,7 +1013,7 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>6</v>
       </c>
       <c r="E9">
@@ -1018,7 +1028,7 @@
       <c r="H9">
         <v>86</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J9" t="s">
@@ -1050,7 +1060,7 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>6</v>
       </c>
       <c r="E10">
@@ -1065,7 +1075,7 @@
       <c r="H10">
         <v>86</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J10" t="s">
@@ -1097,7 +1107,7 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>6</v>
       </c>
       <c r="E11">
@@ -1112,7 +1122,7 @@
       <c r="H11">
         <v>86</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J11" t="s">
@@ -1144,7 +1154,7 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>6</v>
       </c>
       <c r="E12">
@@ -1159,7 +1169,7 @@
       <c r="H12">
         <v>88</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="13" t="s">
         <v>18</v>
       </c>
       <c r="J12" t="s">
@@ -1191,7 +1201,7 @@
       <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>6</v>
       </c>
       <c r="E13">
@@ -1206,7 +1216,7 @@
       <c r="H13">
         <v>88</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J13" t="s">
@@ -1238,7 +1248,7 @@
       <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>6</v>
       </c>
       <c r="E14">
@@ -1253,7 +1263,7 @@
       <c r="H14">
         <v>88</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J14" t="s">
@@ -1285,7 +1295,7 @@
       <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>6</v>
       </c>
       <c r="E15" t="s">
@@ -1300,7 +1310,7 @@
       <c r="H15">
         <v>88</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J15" t="s">
@@ -1332,7 +1342,7 @@
       <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>6</v>
       </c>
       <c r="E16" t="s">
@@ -1347,7 +1357,7 @@
       <c r="H16">
         <v>88</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J16" t="s">
@@ -1379,7 +1389,7 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>6</v>
       </c>
       <c r="E17">
@@ -1394,7 +1404,7 @@
       <c r="H17">
         <v>89</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="13" t="s">
         <v>18</v>
       </c>
       <c r="J17" t="s">
@@ -1426,7 +1436,7 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>6</v>
       </c>
       <c r="E18">
@@ -1441,7 +1451,7 @@
       <c r="H18">
         <v>89</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J18" t="s">
@@ -1473,7 +1483,7 @@
       <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>6</v>
       </c>
       <c r="E19">
@@ -1488,7 +1498,7 @@
       <c r="H19">
         <v>89</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J19" t="s">
@@ -1520,7 +1530,7 @@
       <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>6</v>
       </c>
       <c r="E20" t="s">
@@ -1535,7 +1545,7 @@
       <c r="H20">
         <v>89</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J20" t="s">
@@ -1567,7 +1577,7 @@
       <c r="C21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>6</v>
       </c>
       <c r="E21" t="s">
@@ -1582,7 +1592,7 @@
       <c r="H21">
         <v>89</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J21" t="s">
@@ -1614,7 +1624,7 @@
       <c r="C22" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>1</v>
       </c>
       <c r="E22">
@@ -1629,7 +1639,7 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J22" t="s">
@@ -1661,7 +1671,7 @@
       <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>6</v>
       </c>
       <c r="E23">
@@ -1676,7 +1686,7 @@
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J23" t="s">
@@ -1708,7 +1718,7 @@
       <c r="C24" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>3</v>
       </c>
       <c r="E24">
@@ -1723,7 +1733,7 @@
       <c r="H24">
         <v>3</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J24" t="s">
@@ -1755,7 +1765,7 @@
       <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>5</v>
       </c>
       <c r="E25">
@@ -1770,7 +1780,7 @@
       <c r="H25">
         <v>4</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J25" t="s">
@@ -1802,7 +1812,7 @@
       <c r="C26" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>2</v>
       </c>
       <c r="E26">
@@ -1817,7 +1827,7 @@
       <c r="H26">
         <v>5</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J26" t="s">
@@ -1849,7 +1859,7 @@
       <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>4</v>
       </c>
       <c r="E27">
@@ -1864,7 +1874,7 @@
       <c r="H27">
         <v>6</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J27" t="s">
@@ -1896,7 +1906,7 @@
       <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>2</v>
       </c>
       <c r="E28">
@@ -1911,7 +1921,7 @@
       <c r="H28">
         <v>7</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J28" t="s">
@@ -1943,7 +1953,7 @@
       <c r="C29" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>3</v>
       </c>
       <c r="E29">
@@ -1958,7 +1968,7 @@
       <c r="H29">
         <v>8</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J29" t="s">
@@ -1990,7 +2000,7 @@
       <c r="C30" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>6</v>
       </c>
       <c r="E30">
@@ -2005,7 +2015,7 @@
       <c r="H30">
         <v>9</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J30" t="s">
@@ -2037,7 +2047,7 @@
       <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>2</v>
       </c>
       <c r="E31">
@@ -2052,7 +2062,7 @@
       <c r="H31">
         <v>10</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J31" t="s">
@@ -2084,7 +2094,7 @@
       <c r="C32" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2">
         <v>5</v>
       </c>
       <c r="E32">
@@ -2099,7 +2109,7 @@
       <c r="H32">
         <v>11</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J32" t="s">
@@ -2131,7 +2141,7 @@
       <c r="C33" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2">
         <v>4</v>
       </c>
       <c r="E33">
@@ -2146,7 +2156,7 @@
       <c r="H33">
         <v>12</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J33" t="s">
@@ -2178,7 +2188,7 @@
       <c r="C34" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>6</v>
       </c>
       <c r="E34">
@@ -2193,7 +2203,7 @@
       <c r="H34">
         <v>13</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J34" t="s">
@@ -2225,7 +2235,7 @@
       <c r="C35" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>1</v>
       </c>
       <c r="E35">
@@ -2240,7 +2250,7 @@
       <c r="H35">
         <v>14</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J35" t="s">
@@ -2272,7 +2282,7 @@
       <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>3</v>
       </c>
       <c r="E36">
@@ -2287,7 +2297,7 @@
       <c r="H36">
         <v>15</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J36" t="s">
@@ -2319,7 +2329,7 @@
       <c r="C37" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37">
@@ -2334,7 +2344,7 @@
       <c r="H37">
         <v>16</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J37" t="s">
@@ -2366,7 +2376,7 @@
       <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>4</v>
       </c>
       <c r="E38">
@@ -2381,7 +2391,7 @@
       <c r="H38">
         <v>17</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J38" t="s">
@@ -2413,7 +2423,7 @@
       <c r="C39" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>5</v>
       </c>
       <c r="E39">
@@ -2428,7 +2438,7 @@
       <c r="H39">
         <v>18</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J39" t="s">
@@ -2460,7 +2470,7 @@
       <c r="C40" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>1</v>
       </c>
       <c r="E40">
@@ -2475,7 +2485,7 @@
       <c r="H40">
         <v>1</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J40" t="s">
@@ -2507,7 +2517,7 @@
       <c r="C41" t="s">
         <v>17</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>6</v>
       </c>
       <c r="E41">
@@ -2522,7 +2532,7 @@
       <c r="H41">
         <v>2</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J41" t="s">
@@ -2554,7 +2564,7 @@
       <c r="C42" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>3</v>
       </c>
       <c r="E42">
@@ -2569,7 +2579,7 @@
       <c r="H42">
         <v>3</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J42" t="s">
@@ -2601,7 +2611,7 @@
       <c r="C43" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>5</v>
       </c>
       <c r="E43">
@@ -2616,7 +2626,7 @@
       <c r="H43">
         <v>4</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J43" t="s">
@@ -2648,7 +2658,7 @@
       <c r="C44" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>2</v>
       </c>
       <c r="E44">
@@ -2663,7 +2673,7 @@
       <c r="H44">
         <v>5</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J44" t="s">
@@ -2695,7 +2705,7 @@
       <c r="C45" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>4</v>
       </c>
       <c r="E45">
@@ -2710,7 +2720,7 @@
       <c r="H45">
         <v>6</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J45" t="s">
@@ -2742,7 +2752,7 @@
       <c r="C46" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2">
         <v>2</v>
       </c>
       <c r="E46">
@@ -2757,7 +2767,7 @@
       <c r="H46">
         <v>7</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J46" t="s">
@@ -2789,7 +2799,7 @@
       <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2">
         <v>3</v>
       </c>
       <c r="E47">
@@ -2804,7 +2814,7 @@
       <c r="H47">
         <v>8</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J47" t="s">
@@ -2836,7 +2846,7 @@
       <c r="C48" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2">
         <v>6</v>
       </c>
       <c r="E48">
@@ -2851,7 +2861,7 @@
       <c r="H48">
         <v>9</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J48" t="s">
@@ -2883,7 +2893,7 @@
       <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2">
         <v>2</v>
       </c>
       <c r="E49">
@@ -2898,7 +2908,7 @@
       <c r="H49">
         <v>10</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J49" t="s">
@@ -2930,7 +2940,7 @@
       <c r="C50" t="s">
         <v>17</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2">
         <v>5</v>
       </c>
       <c r="E50">
@@ -2945,7 +2955,7 @@
       <c r="H50">
         <v>11</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J50" t="s">
@@ -2977,7 +2987,7 @@
       <c r="C51" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2">
         <v>4</v>
       </c>
       <c r="E51">
@@ -2992,7 +3002,7 @@
       <c r="H51">
         <v>12</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J51" t="s">
@@ -3024,7 +3034,7 @@
       <c r="C52" t="s">
         <v>17</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>6</v>
       </c>
       <c r="E52">
@@ -3039,7 +3049,7 @@
       <c r="H52">
         <v>13</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J52" t="s">
@@ -3071,7 +3081,7 @@
       <c r="C53" t="s">
         <v>17</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>1</v>
       </c>
       <c r="E53">
@@ -3086,7 +3096,7 @@
       <c r="H53">
         <v>14</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I53" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J53" t="s">
@@ -3118,7 +3128,7 @@
       <c r="C54" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2">
         <v>3</v>
       </c>
       <c r="E54">
@@ -3133,7 +3143,7 @@
       <c r="H54">
         <v>15</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I54" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J54" t="s">
@@ -3165,7 +3175,7 @@
       <c r="C55" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="2">
         <v>1</v>
       </c>
       <c r="E55">
@@ -3180,7 +3190,7 @@
       <c r="H55">
         <v>16</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J55" t="s">
@@ -3212,7 +3222,7 @@
       <c r="C56" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="2">
         <v>4</v>
       </c>
       <c r="E56">
@@ -3227,7 +3237,7 @@
       <c r="H56">
         <v>17</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I56" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J56" t="s">
@@ -3259,7 +3269,7 @@
       <c r="C57" t="s">
         <v>17</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="2">
         <v>5</v>
       </c>
       <c r="E57">
@@ -3274,7 +3284,7 @@
       <c r="H57">
         <v>18</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I57" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J57" t="s">
@@ -3306,7 +3316,7 @@
       <c r="C58" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="2">
         <v>4</v>
       </c>
       <c r="E58">
@@ -3321,7 +3331,7 @@
       <c r="H58">
         <v>19</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I58" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J58" t="s">
@@ -3353,7 +3363,7 @@
       <c r="C59" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2">
         <v>2</v>
       </c>
       <c r="E59">
@@ -3368,7 +3378,7 @@
       <c r="H59">
         <v>20</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I59" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J59" t="s">
@@ -3400,7 +3410,7 @@
       <c r="C60" t="s">
         <v>16</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2">
         <v>5</v>
       </c>
       <c r="E60">
@@ -3415,7 +3425,7 @@
       <c r="H60">
         <v>21</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J60" t="s">
@@ -3447,7 +3457,7 @@
       <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61">
@@ -3462,7 +3472,7 @@
       <c r="H61">
         <v>22</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J61" t="s">
@@ -3494,7 +3504,7 @@
       <c r="C62" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="2">
         <v>5</v>
       </c>
       <c r="E62">
@@ -3509,7 +3519,7 @@
       <c r="H62">
         <v>23</v>
       </c>
-      <c r="I62" t="s">
+      <c r="I62" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J62" t="s">
@@ -3541,7 +3551,7 @@
       <c r="C63" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <v>3</v>
       </c>
       <c r="E63">
@@ -3556,7 +3566,7 @@
       <c r="H63">
         <v>24</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J63" t="s">
@@ -3588,7 +3598,7 @@
       <c r="C64" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="2">
         <v>6</v>
       </c>
       <c r="E64">
@@ -3603,7 +3613,7 @@
       <c r="H64">
         <v>25</v>
       </c>
-      <c r="I64" t="s">
+      <c r="I64" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J64" t="s">
@@ -3635,7 +3645,7 @@
       <c r="C65" t="s">
         <v>16</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="2">
         <v>4</v>
       </c>
       <c r="E65">
@@ -3650,7 +3660,7 @@
       <c r="H65">
         <v>26</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I65" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J65" t="s">
@@ -3682,7 +3692,7 @@
       <c r="C66" t="s">
         <v>16</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="2">
         <v>1</v>
       </c>
       <c r="E66">
@@ -3697,7 +3707,7 @@
       <c r="H66">
         <v>27</v>
       </c>
-      <c r="I66" t="s">
+      <c r="I66" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J66" t="s">
@@ -3729,7 +3739,7 @@
       <c r="C67" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2">
         <v>3</v>
       </c>
       <c r="E67">
@@ -3744,7 +3754,7 @@
       <c r="H67">
         <v>28</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J67" t="s">
@@ -3776,7 +3786,7 @@
       <c r="C68" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="2">
         <v>1</v>
       </c>
       <c r="E68">
@@ -3791,7 +3801,7 @@
       <c r="H68">
         <v>29</v>
       </c>
-      <c r="I68" t="s">
+      <c r="I68" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J68" t="s">
@@ -3823,7 +3833,7 @@
       <c r="C69" t="s">
         <v>16</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="2">
         <v>6</v>
       </c>
       <c r="E69">
@@ -3838,7 +3848,7 @@
       <c r="H69">
         <v>30</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I69" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J69" t="s">
@@ -3870,7 +3880,7 @@
       <c r="C70" t="s">
         <v>16</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="2">
         <v>2</v>
       </c>
       <c r="E70">
@@ -3885,7 +3895,7 @@
       <c r="H70">
         <v>31</v>
       </c>
-      <c r="I70" t="s">
+      <c r="I70" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J70" t="s">
@@ -3917,7 +3927,7 @@
       <c r="C71" t="s">
         <v>16</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="2">
         <v>6</v>
       </c>
       <c r="E71">
@@ -3932,7 +3942,7 @@
       <c r="H71">
         <v>32</v>
       </c>
-      <c r="I71" t="s">
+      <c r="I71" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J71" t="s">
@@ -3964,7 +3974,7 @@
       <c r="C72" t="s">
         <v>16</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="2">
         <v>4</v>
       </c>
       <c r="E72">
@@ -3979,7 +3989,7 @@
       <c r="H72">
         <v>33</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J72" t="s">
@@ -4011,7 +4021,7 @@
       <c r="C73" t="s">
         <v>16</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="2">
         <v>5</v>
       </c>
       <c r="E73">
@@ -4026,7 +4036,7 @@
       <c r="H73">
         <v>34</v>
       </c>
-      <c r="I73" t="s">
+      <c r="I73" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J73" t="s">
@@ -4058,7 +4068,7 @@
       <c r="C74" t="s">
         <v>16</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="2">
         <v>3</v>
       </c>
       <c r="E74">
@@ -4073,7 +4083,7 @@
       <c r="H74">
         <v>35</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J74" t="s">
@@ -4105,7 +4115,7 @@
       <c r="C75" t="s">
         <v>16</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="2">
         <v>2</v>
       </c>
       <c r="E75">
@@ -4120,7 +4130,7 @@
       <c r="H75">
         <v>36</v>
       </c>
-      <c r="I75" t="s">
+      <c r="I75" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J75" t="s">
@@ -4152,7 +4162,7 @@
       <c r="C76" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="2">
         <v>4</v>
       </c>
       <c r="E76">
@@ -4167,7 +4177,7 @@
       <c r="H76">
         <v>19</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I76" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J76" t="s">
@@ -4199,7 +4209,7 @@
       <c r="C77" t="s">
         <v>17</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="2">
         <v>2</v>
       </c>
       <c r="E77">
@@ -4214,7 +4224,7 @@
       <c r="H77">
         <v>20</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I77" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J77" t="s">
@@ -4246,7 +4256,7 @@
       <c r="C78" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="2">
         <v>5</v>
       </c>
       <c r="E78">
@@ -4261,7 +4271,7 @@
       <c r="H78">
         <v>21</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J78" t="s">
@@ -4293,7 +4303,7 @@
       <c r="C79" t="s">
         <v>17</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="2">
         <v>1</v>
       </c>
       <c r="E79">
@@ -4308,7 +4318,7 @@
       <c r="H79">
         <v>22</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I79" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J79" t="s">
@@ -4340,7 +4350,7 @@
       <c r="C80" t="s">
         <v>17</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="2">
         <v>5</v>
       </c>
       <c r="E80">
@@ -4355,7 +4365,7 @@
       <c r="H80">
         <v>23</v>
       </c>
-      <c r="I80" t="s">
+      <c r="I80" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J80" t="s">
@@ -4387,7 +4397,7 @@
       <c r="C81" t="s">
         <v>17</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="2">
         <v>3</v>
       </c>
       <c r="E81">
@@ -4402,7 +4412,7 @@
       <c r="H81">
         <v>24</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I81" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J81" t="s">
@@ -4434,7 +4444,7 @@
       <c r="C82" t="s">
         <v>17</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="2">
         <v>6</v>
       </c>
       <c r="E82">
@@ -4449,7 +4459,7 @@
       <c r="H82">
         <v>25</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I82" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J82" t="s">
@@ -4481,7 +4491,7 @@
       <c r="C83" t="s">
         <v>17</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="2">
         <v>4</v>
       </c>
       <c r="E83">
@@ -4496,7 +4506,7 @@
       <c r="H83">
         <v>26</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I83" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J83" t="s">
@@ -4528,7 +4538,7 @@
       <c r="C84" t="s">
         <v>17</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="2">
         <v>1</v>
       </c>
       <c r="E84">
@@ -4543,7 +4553,7 @@
       <c r="H84">
         <v>27</v>
       </c>
-      <c r="I84" t="s">
+      <c r="I84" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J84" t="s">
@@ -4575,7 +4585,7 @@
       <c r="C85" t="s">
         <v>17</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="2">
         <v>3</v>
       </c>
       <c r="E85">
@@ -4590,7 +4600,7 @@
       <c r="H85">
         <v>28</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I85" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J85" t="s">
@@ -4622,7 +4632,7 @@
       <c r="C86" t="s">
         <v>17</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="2">
         <v>1</v>
       </c>
       <c r="E86">
@@ -4637,7 +4647,7 @@
       <c r="H86">
         <v>29</v>
       </c>
-      <c r="I86" t="s">
+      <c r="I86" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J86" t="s">
@@ -4669,7 +4679,7 @@
       <c r="C87" t="s">
         <v>17</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="2">
         <v>6</v>
       </c>
       <c r="E87">
@@ -4684,7 +4694,7 @@
       <c r="H87">
         <v>30</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I87" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J87" t="s">
@@ -4716,7 +4726,7 @@
       <c r="C88" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="2">
         <v>2</v>
       </c>
       <c r="E88">
@@ -4731,7 +4741,7 @@
       <c r="H88">
         <v>31</v>
       </c>
-      <c r="I88" t="s">
+      <c r="I88" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J88" t="s">
@@ -4763,7 +4773,7 @@
       <c r="C89" t="s">
         <v>17</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="2">
         <v>6</v>
       </c>
       <c r="E89">
@@ -4778,7 +4788,7 @@
       <c r="H89">
         <v>32</v>
       </c>
-      <c r="I89" t="s">
+      <c r="I89" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J89" t="s">
@@ -4810,7 +4820,7 @@
       <c r="C90" t="s">
         <v>17</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="2">
         <v>4</v>
       </c>
       <c r="E90">
@@ -4825,7 +4835,7 @@
       <c r="H90">
         <v>33</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I90" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J90" t="s">
@@ -4857,7 +4867,7 @@
       <c r="C91" t="s">
         <v>17</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="2">
         <v>5</v>
       </c>
       <c r="E91">
@@ -4872,7 +4882,7 @@
       <c r="H91">
         <v>34</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I91" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J91" t="s">
@@ -4904,7 +4914,7 @@
       <c r="C92" t="s">
         <v>17</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D92" s="2">
         <v>3</v>
       </c>
       <c r="E92">
@@ -4919,7 +4929,7 @@
       <c r="H92">
         <v>35</v>
       </c>
-      <c r="I92" t="s">
+      <c r="I92" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J92" t="s">
@@ -4951,7 +4961,7 @@
       <c r="C93" t="s">
         <v>17</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D93" s="2">
         <v>2</v>
       </c>
       <c r="E93">
@@ -4966,7 +4976,7 @@
       <c r="H93">
         <v>36</v>
       </c>
-      <c r="I93" t="s">
+      <c r="I93" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J93" t="s">
@@ -4998,7 +5008,7 @@
       <c r="C94" t="s">
         <v>16</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D94" s="2">
         <v>6</v>
       </c>
       <c r="E94">
@@ -5013,7 +5023,7 @@
       <c r="H94">
         <v>37</v>
       </c>
-      <c r="I94" t="s">
+      <c r="I94" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J94" t="s">
@@ -5045,7 +5055,7 @@
       <c r="C95" t="s">
         <v>16</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D95" s="2">
         <v>3</v>
       </c>
       <c r="E95">
@@ -5060,7 +5070,7 @@
       <c r="H95">
         <v>38</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I95" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J95" t="s">
@@ -5092,7 +5102,7 @@
       <c r="C96" t="s">
         <v>16</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="2">
         <v>1</v>
       </c>
       <c r="E96">
@@ -5107,7 +5117,7 @@
       <c r="H96">
         <v>39</v>
       </c>
-      <c r="I96" t="s">
+      <c r="I96" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J96" t="s">
@@ -5139,7 +5149,7 @@
       <c r="C97" t="s">
         <v>16</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="2">
         <v>1</v>
       </c>
       <c r="E97">
@@ -5154,7 +5164,7 @@
       <c r="H97">
         <v>40</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I97" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J97" t="s">
@@ -5186,7 +5196,7 @@
       <c r="C98" t="s">
         <v>16</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="2">
         <v>6</v>
       </c>
       <c r="E98">
@@ -5201,7 +5211,7 @@
       <c r="H98">
         <v>41</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J98" t="s">
@@ -5233,7 +5243,7 @@
       <c r="C99" t="s">
         <v>16</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="2">
         <v>4</v>
       </c>
       <c r="E99">
@@ -5248,7 +5258,7 @@
       <c r="H99">
         <v>42</v>
       </c>
-      <c r="I99" t="s">
+      <c r="I99" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J99" t="s">
@@ -5280,7 +5290,7 @@
       <c r="C100" t="s">
         <v>16</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="2">
         <v>3</v>
       </c>
       <c r="E100">
@@ -5295,7 +5305,7 @@
       <c r="H100">
         <v>43</v>
       </c>
-      <c r="I100" t="s">
+      <c r="I100" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J100" t="s">
@@ -5327,7 +5337,7 @@
       <c r="C101" t="s">
         <v>16</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="2">
         <v>1</v>
       </c>
       <c r="E101">
@@ -5342,7 +5352,7 @@
       <c r="H101">
         <v>44</v>
       </c>
-      <c r="I101" t="s">
+      <c r="I101" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J101" t="s">
@@ -5374,7 +5384,7 @@
       <c r="C102" t="s">
         <v>16</v>
       </c>
-      <c r="D102" s="3">
+      <c r="D102" s="2">
         <v>5</v>
       </c>
       <c r="E102">
@@ -5389,7 +5399,7 @@
       <c r="H102">
         <v>45</v>
       </c>
-      <c r="I102" t="s">
+      <c r="I102" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J102" t="s">
@@ -5421,7 +5431,7 @@
       <c r="C103" t="s">
         <v>16</v>
       </c>
-      <c r="D103" s="3">
+      <c r="D103" s="2">
         <v>5</v>
       </c>
       <c r="E103">
@@ -5436,7 +5446,7 @@
       <c r="H103">
         <v>46</v>
       </c>
-      <c r="I103" t="s">
+      <c r="I103" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J103" t="s">
@@ -5468,7 +5478,7 @@
       <c r="C104" t="s">
         <v>16</v>
       </c>
-      <c r="D104" s="3">
+      <c r="D104" s="2">
         <v>4</v>
       </c>
       <c r="E104">
@@ -5483,7 +5493,7 @@
       <c r="H104">
         <v>47</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J104" t="s">
@@ -5515,7 +5525,7 @@
       <c r="C105" t="s">
         <v>16</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="2">
         <v>2</v>
       </c>
       <c r="E105">
@@ -5530,7 +5540,7 @@
       <c r="H105">
         <v>48</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J105" t="s">
@@ -5562,7 +5572,7 @@
       <c r="C106" t="s">
         <v>16</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D106" s="2">
         <v>2</v>
       </c>
       <c r="E106">
@@ -5577,7 +5587,7 @@
       <c r="H106">
         <v>49</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J106" t="s">
@@ -5609,7 +5619,7 @@
       <c r="C107" t="s">
         <v>16</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="2">
         <v>5</v>
       </c>
       <c r="E107">
@@ -5624,7 +5634,7 @@
       <c r="H107">
         <v>50</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J107" t="s">
@@ -5656,7 +5666,7 @@
       <c r="C108" t="s">
         <v>16</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="2">
         <v>3</v>
       </c>
       <c r="E108">
@@ -5671,7 +5681,7 @@
       <c r="H108">
         <v>51</v>
       </c>
-      <c r="I108" t="s">
+      <c r="I108" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J108" t="s">
@@ -5703,7 +5713,7 @@
       <c r="C109" t="s">
         <v>16</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D109" s="2">
         <v>4</v>
       </c>
       <c r="E109">
@@ -5718,7 +5728,7 @@
       <c r="H109">
         <v>52</v>
       </c>
-      <c r="I109" t="s">
+      <c r="I109" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J109" t="s">
@@ -5750,7 +5760,7 @@
       <c r="C110" t="s">
         <v>16</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D110" s="2">
         <v>2</v>
       </c>
       <c r="E110">
@@ -5765,7 +5775,7 @@
       <c r="H110">
         <v>53</v>
       </c>
-      <c r="I110" t="s">
+      <c r="I110" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J110" t="s">
@@ -5797,7 +5807,7 @@
       <c r="C111" t="s">
         <v>16</v>
       </c>
-      <c r="D111" s="3">
+      <c r="D111" s="2">
         <v>6</v>
       </c>
       <c r="E111">
@@ -5812,7 +5822,7 @@
       <c r="H111">
         <v>54</v>
       </c>
-      <c r="I111" t="s">
+      <c r="I111" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J111" t="s">
@@ -5844,7 +5854,7 @@
       <c r="C112" t="s">
         <v>16</v>
       </c>
-      <c r="D112" s="3">
+      <c r="D112" s="2">
         <v>1</v>
       </c>
       <c r="E112">
@@ -5859,7 +5869,7 @@
       <c r="H112">
         <v>55</v>
       </c>
-      <c r="I112" t="s">
+      <c r="I112" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J112" t="s">
@@ -5891,7 +5901,7 @@
       <c r="C113" t="s">
         <v>16</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="2">
         <v>5</v>
       </c>
       <c r="E113">
@@ -5906,7 +5916,7 @@
       <c r="H113">
         <v>56</v>
       </c>
-      <c r="I113" t="s">
+      <c r="I113" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J113" t="s">
@@ -5938,7 +5948,7 @@
       <c r="C114" t="s">
         <v>16</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="2">
         <v>4</v>
       </c>
       <c r="E114">
@@ -5953,7 +5963,7 @@
       <c r="H114">
         <v>57</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I114" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J114" t="s">
@@ -5985,7 +5995,7 @@
       <c r="C115" t="s">
         <v>16</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="2">
         <v>6</v>
       </c>
       <c r="E115">
@@ -6000,7 +6010,7 @@
       <c r="H115">
         <v>58</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I115" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J115" t="s">
@@ -6032,7 +6042,7 @@
       <c r="C116" t="s">
         <v>16</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="2">
         <v>3</v>
       </c>
       <c r="E116">
@@ -6047,7 +6057,7 @@
       <c r="H116">
         <v>59</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I116" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J116" t="s">
@@ -6079,7 +6089,7 @@
       <c r="C117" t="s">
         <v>16</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D117" s="2">
         <v>2</v>
       </c>
       <c r="E117">
@@ -6094,7 +6104,7 @@
       <c r="H117">
         <v>60</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I117" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J117" t="s">
@@ -6126,7 +6136,7 @@
       <c r="C118" t="s">
         <v>16</v>
       </c>
-      <c r="D118" s="3">
+      <c r="D118" s="2">
         <v>5</v>
       </c>
       <c r="E118">
@@ -6141,7 +6151,7 @@
       <c r="H118">
         <v>61</v>
       </c>
-      <c r="I118" t="s">
+      <c r="I118" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J118" t="s">
@@ -6173,7 +6183,7 @@
       <c r="C119" t="s">
         <v>16</v>
       </c>
-      <c r="D119" s="3">
+      <c r="D119" s="2">
         <v>1</v>
       </c>
       <c r="E119">
@@ -6188,7 +6198,7 @@
       <c r="H119">
         <v>62</v>
       </c>
-      <c r="I119" t="s">
+      <c r="I119" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J119" t="s">
@@ -6220,7 +6230,7 @@
       <c r="C120" t="s">
         <v>16</v>
       </c>
-      <c r="D120" s="3">
+      <c r="D120" s="2">
         <v>4</v>
       </c>
       <c r="E120">
@@ -6235,7 +6245,7 @@
       <c r="H120">
         <v>63</v>
       </c>
-      <c r="I120" t="s">
+      <c r="I120" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J120" t="s">
@@ -6267,7 +6277,7 @@
       <c r="C121" t="s">
         <v>16</v>
       </c>
-      <c r="D121" s="3">
+      <c r="D121" s="2">
         <v>2</v>
       </c>
       <c r="E121">
@@ -6282,7 +6292,7 @@
       <c r="H121">
         <v>64</v>
       </c>
-      <c r="I121" t="s">
+      <c r="I121" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J121" t="s">
@@ -6314,7 +6324,7 @@
       <c r="C122" t="s">
         <v>16</v>
       </c>
-      <c r="D122" s="3">
+      <c r="D122" s="2">
         <v>6</v>
       </c>
       <c r="E122">
@@ -6329,7 +6339,7 @@
       <c r="H122">
         <v>65</v>
       </c>
-      <c r="I122" t="s">
+      <c r="I122" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J122" t="s">
@@ -6361,7 +6371,7 @@
       <c r="C123" t="s">
         <v>16</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D123" s="2">
         <v>3</v>
       </c>
       <c r="E123">
@@ -6376,7 +6386,7 @@
       <c r="H123">
         <v>66</v>
       </c>
-      <c r="I123" t="s">
+      <c r="I123" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J123" t="s">
@@ -6408,7 +6418,7 @@
       <c r="C124" t="s">
         <v>16</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D124" s="2">
         <v>5</v>
       </c>
       <c r="E124">
@@ -6423,7 +6433,7 @@
       <c r="H124">
         <v>67</v>
       </c>
-      <c r="I124" t="s">
+      <c r="I124" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J124" t="s">
@@ -6455,7 +6465,7 @@
       <c r="C125" t="s">
         <v>16</v>
       </c>
-      <c r="D125" s="3">
+      <c r="D125" s="2">
         <v>4</v>
       </c>
       <c r="E125">
@@ -6470,7 +6480,7 @@
       <c r="H125">
         <v>68</v>
       </c>
-      <c r="I125" t="s">
+      <c r="I125" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J125" t="s">
@@ -6502,7 +6512,7 @@
       <c r="C126" t="s">
         <v>16</v>
       </c>
-      <c r="D126" s="3">
+      <c r="D126" s="2">
         <v>1</v>
       </c>
       <c r="E126">
@@ -6517,7 +6527,7 @@
       <c r="H126">
         <v>69</v>
       </c>
-      <c r="I126" t="s">
+      <c r="I126" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J126" t="s">
@@ -6549,7 +6559,7 @@
       <c r="C127" t="s">
         <v>16</v>
       </c>
-      <c r="D127" s="3">
+      <c r="D127" s="2">
         <v>6</v>
       </c>
       <c r="E127">
@@ -6564,7 +6574,7 @@
       <c r="H127">
         <v>70</v>
       </c>
-      <c r="I127" t="s">
+      <c r="I127" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J127" t="s">
@@ -6596,7 +6606,7 @@
       <c r="C128" t="s">
         <v>16</v>
       </c>
-      <c r="D128" s="3">
+      <c r="D128" s="2">
         <v>2</v>
       </c>
       <c r="E128">
@@ -6611,7 +6621,7 @@
       <c r="H128">
         <v>71</v>
       </c>
-      <c r="I128" t="s">
+      <c r="I128" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J128" t="s">
@@ -6643,7 +6653,7 @@
       <c r="C129" t="s">
         <v>16</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D129" s="2">
         <v>3</v>
       </c>
       <c r="E129">
@@ -6658,7 +6668,7 @@
       <c r="H129">
         <v>72</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I129" s="13" t="s">
         <v>16</v>
       </c>
       <c r="J129" t="s">
@@ -6690,7 +6700,7 @@
       <c r="C130" t="s">
         <v>16</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D130" s="2">
         <v>4</v>
       </c>
       <c r="E130">
@@ -6705,7 +6715,7 @@
       <c r="H130">
         <v>73</v>
       </c>
-      <c r="I130" s="1" t="s">
+      <c r="I130" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J130" t="s">
@@ -6737,7 +6747,7 @@
       <c r="C131" t="s">
         <v>16</v>
       </c>
-      <c r="D131" s="3">
+      <c r="D131" s="2">
         <v>1</v>
       </c>
       <c r="E131">
@@ -6752,7 +6762,7 @@
       <c r="H131">
         <v>74</v>
       </c>
-      <c r="I131" s="1" t="s">
+      <c r="I131" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J131" t="s">
@@ -6784,7 +6794,7 @@
       <c r="C132" t="s">
         <v>16</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D132" s="2">
         <v>1</v>
       </c>
       <c r="E132">
@@ -6799,7 +6809,7 @@
       <c r="H132">
         <v>75</v>
       </c>
-      <c r="I132" s="1" t="s">
+      <c r="I132" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J132" t="s">
@@ -6831,7 +6841,7 @@
       <c r="C133" t="s">
         <v>16</v>
       </c>
-      <c r="D133" s="3">
+      <c r="D133" s="2">
         <v>3</v>
       </c>
       <c r="E133">
@@ -6846,7 +6856,7 @@
       <c r="H133">
         <v>76</v>
       </c>
-      <c r="I133" s="1" t="s">
+      <c r="I133" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J133" t="s">
@@ -6878,7 +6888,7 @@
       <c r="C134" t="s">
         <v>16</v>
       </c>
-      <c r="D134" s="3">
+      <c r="D134" s="2">
         <v>1</v>
       </c>
       <c r="E134">
@@ -6893,7 +6903,7 @@
       <c r="H134">
         <v>77</v>
       </c>
-      <c r="I134" s="1" t="s">
+      <c r="I134" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J134" t="s">
@@ -6925,7 +6935,7 @@
       <c r="C135" t="s">
         <v>16</v>
       </c>
-      <c r="D135" s="3">
+      <c r="D135" s="2">
         <v>3</v>
       </c>
       <c r="E135">
@@ -6940,7 +6950,7 @@
       <c r="H135">
         <v>78</v>
       </c>
-      <c r="I135" s="1" t="s">
+      <c r="I135" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J135" t="s">
@@ -6972,7 +6982,7 @@
       <c r="C136" t="s">
         <v>16</v>
       </c>
-      <c r="D136" s="3">
+      <c r="D136" s="2">
         <v>5</v>
       </c>
       <c r="E136">
@@ -6987,7 +6997,7 @@
       <c r="H136">
         <v>79</v>
       </c>
-      <c r="I136" s="1" t="s">
+      <c r="I136" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J136" t="s">
@@ -7019,7 +7029,7 @@
       <c r="C137" t="s">
         <v>16</v>
       </c>
-      <c r="D137" s="3">
+      <c r="D137" s="2">
         <v>3</v>
       </c>
       <c r="E137">
@@ -7034,7 +7044,7 @@
       <c r="H137">
         <v>80</v>
       </c>
-      <c r="I137" s="1" t="s">
+      <c r="I137" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J137" t="s">
@@ -7066,7 +7076,7 @@
       <c r="C138" t="s">
         <v>16</v>
       </c>
-      <c r="D138" s="3">
+      <c r="D138" s="2">
         <v>5</v>
       </c>
       <c r="E138">
@@ -7081,7 +7091,7 @@
       <c r="H138">
         <v>81</v>
       </c>
-      <c r="I138" s="1" t="s">
+      <c r="I138" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J138" t="s">
@@ -7113,7 +7123,7 @@
       <c r="C139" t="s">
         <v>16</v>
       </c>
-      <c r="D139" s="3">
+      <c r="D139" s="2">
         <v>5</v>
       </c>
       <c r="E139">
@@ -7128,7 +7138,7 @@
       <c r="H139">
         <v>82</v>
       </c>
-      <c r="I139" s="1" t="s">
+      <c r="I139" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J139" t="s">
@@ -7160,7 +7170,7 @@
       <c r="C140" t="s">
         <v>16</v>
       </c>
-      <c r="D140" s="3">
+      <c r="D140" s="2">
         <v>3</v>
       </c>
       <c r="E140">
@@ -7175,7 +7185,7 @@
       <c r="H140">
         <v>83</v>
       </c>
-      <c r="I140" s="1" t="s">
+      <c r="I140" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J140" t="s">
@@ -7207,7 +7217,7 @@
       <c r="C141" t="s">
         <v>16</v>
       </c>
-      <c r="D141" s="3">
+      <c r="D141" s="2">
         <v>5</v>
       </c>
       <c r="E141">
@@ -7222,7 +7232,7 @@
       <c r="H141">
         <v>84</v>
       </c>
-      <c r="I141" s="1" t="s">
+      <c r="I141" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J141" t="s">
@@ -7254,7 +7264,7 @@
       <c r="C142" t="s">
         <v>16</v>
       </c>
-      <c r="D142" s="3">
+      <c r="D142" s="2">
         <v>1</v>
       </c>
       <c r="E142">
@@ -7269,7 +7279,7 @@
       <c r="H142">
         <v>87</v>
       </c>
-      <c r="I142" s="1" t="s">
+      <c r="I142" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J142" t="s">
@@ -7301,7 +7311,7 @@
       <c r="C143" t="s">
         <v>16</v>
       </c>
-      <c r="D143" s="3">
+      <c r="D143" s="2">
         <v>1</v>
       </c>
       <c r="E143">
@@ -7316,7 +7326,7 @@
       <c r="H143">
         <v>90</v>
       </c>
-      <c r="I143" s="1" t="s">
+      <c r="I143" s="14" t="s">
         <v>32</v>
       </c>
       <c r="J143" t="s">
@@ -7348,7 +7358,7 @@
       <c r="C144" t="s">
         <v>16</v>
       </c>
-      <c r="D144" s="3">
+      <c r="D144" s="2">
         <v>2</v>
       </c>
       <c r="E144">
@@ -7363,7 +7373,7 @@
       <c r="H144">
         <v>91</v>
       </c>
-      <c r="I144" t="s">
+      <c r="I144" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J144" t="s">
@@ -7395,7 +7405,7 @@
       <c r="C145" t="s">
         <v>16</v>
       </c>
-      <c r="D145" s="3">
+      <c r="D145" s="2">
         <v>3</v>
       </c>
       <c r="E145">
@@ -7410,7 +7420,7 @@
       <c r="H145">
         <v>92</v>
       </c>
-      <c r="I145" t="s">
+      <c r="I145" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J145" t="s">
@@ -7442,7 +7452,7 @@
       <c r="C146" t="s">
         <v>16</v>
       </c>
-      <c r="D146" s="3">
+      <c r="D146" s="2">
         <v>3</v>
       </c>
       <c r="E146">
@@ -7457,7 +7467,7 @@
       <c r="H146">
         <v>93</v>
       </c>
-      <c r="I146" t="s">
+      <c r="I146" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J146" t="s">
@@ -7489,7 +7499,7 @@
       <c r="C147" t="s">
         <v>16</v>
       </c>
-      <c r="D147" s="3">
+      <c r="D147" s="2">
         <v>4</v>
       </c>
       <c r="E147">
@@ -7504,7 +7514,7 @@
       <c r="H147">
         <v>94</v>
       </c>
-      <c r="I147" t="s">
+      <c r="I147" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J147" t="s">
@@ -7536,7 +7546,7 @@
       <c r="C148" t="s">
         <v>16</v>
       </c>
-      <c r="D148" s="3">
+      <c r="D148" s="2">
         <v>1</v>
       </c>
       <c r="E148">
@@ -7551,7 +7561,7 @@
       <c r="H148">
         <v>95</v>
       </c>
-      <c r="I148" t="s">
+      <c r="I148" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J148" t="s">
@@ -7583,7 +7593,7 @@
       <c r="C149" t="s">
         <v>16</v>
       </c>
-      <c r="D149" s="3">
+      <c r="D149" s="2">
         <v>2</v>
       </c>
       <c r="E149">
@@ -7598,7 +7608,7 @@
       <c r="H149">
         <v>96</v>
       </c>
-      <c r="I149" t="s">
+      <c r="I149" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J149" t="s">
@@ -7630,7 +7640,7 @@
       <c r="C150" t="s">
         <v>16</v>
       </c>
-      <c r="D150" s="3">
+      <c r="D150" s="2">
         <v>1</v>
       </c>
       <c r="E150">
@@ -7645,7 +7655,7 @@
       <c r="H150">
         <v>97</v>
       </c>
-      <c r="I150" t="s">
+      <c r="I150" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J150" t="s">
@@ -7677,7 +7687,7 @@
       <c r="C151" t="s">
         <v>16</v>
       </c>
-      <c r="D151" s="3">
+      <c r="D151" s="2">
         <v>4</v>
       </c>
       <c r="E151">
@@ -7692,7 +7702,7 @@
       <c r="H151">
         <v>98</v>
       </c>
-      <c r="I151" t="s">
+      <c r="I151" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J151" t="s">
@@ -7724,7 +7734,7 @@
       <c r="C152" t="s">
         <v>16</v>
       </c>
-      <c r="D152" s="3">
+      <c r="D152" s="2">
         <v>2</v>
       </c>
       <c r="E152">
@@ -7739,7 +7749,7 @@
       <c r="H152">
         <v>99</v>
       </c>
-      <c r="I152" t="s">
+      <c r="I152" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J152" t="s">
@@ -7771,7 +7781,7 @@
       <c r="C153" t="s">
         <v>16</v>
       </c>
-      <c r="D153" s="3">
+      <c r="D153" s="2">
         <v>1</v>
       </c>
       <c r="E153">
@@ -7786,7 +7796,7 @@
       <c r="H153">
         <v>100</v>
       </c>
-      <c r="I153" t="s">
+      <c r="I153" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J153" t="s">
@@ -7818,7 +7828,7 @@
       <c r="C154" t="s">
         <v>16</v>
       </c>
-      <c r="D154" s="3">
+      <c r="D154" s="2">
         <v>4</v>
       </c>
       <c r="E154">
@@ -7833,7 +7843,7 @@
       <c r="H154">
         <v>101</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I154" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J154" t="s">
@@ -7865,7 +7875,7 @@
       <c r="C155" t="s">
         <v>16</v>
       </c>
-      <c r="D155" s="3">
+      <c r="D155" s="2">
         <v>3</v>
       </c>
       <c r="E155">
@@ -7880,7 +7890,7 @@
       <c r="H155">
         <v>102</v>
       </c>
-      <c r="I155" t="s">
+      <c r="I155" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J155" t="s">
@@ -7912,7 +7922,7 @@
       <c r="C156" t="s">
         <v>16</v>
       </c>
-      <c r="D156" s="3">
+      <c r="D156" s="2">
         <v>2</v>
       </c>
       <c r="E156">
@@ -7927,7 +7937,7 @@
       <c r="H156">
         <v>91</v>
       </c>
-      <c r="I156" t="s">
+      <c r="I156" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J156" t="s">
@@ -7959,7 +7969,7 @@
       <c r="C157" t="s">
         <v>16</v>
       </c>
-      <c r="D157" s="3">
+      <c r="D157" s="2">
         <v>3</v>
       </c>
       <c r="E157">
@@ -7974,7 +7984,7 @@
       <c r="H157">
         <v>92</v>
       </c>
-      <c r="I157" t="s">
+      <c r="I157" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J157" t="s">
@@ -8006,7 +8016,7 @@
       <c r="C158" t="s">
         <v>16</v>
       </c>
-      <c r="D158" s="3">
+      <c r="D158" s="2">
         <v>3</v>
       </c>
       <c r="E158">
@@ -8021,7 +8031,7 @@
       <c r="H158">
         <v>93</v>
       </c>
-      <c r="I158" t="s">
+      <c r="I158" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J158" t="s">
@@ -8053,7 +8063,7 @@
       <c r="C159" t="s">
         <v>16</v>
       </c>
-      <c r="D159" s="3">
+      <c r="D159" s="2">
         <v>4</v>
       </c>
       <c r="E159">
@@ -8068,7 +8078,7 @@
       <c r="H159">
         <v>94</v>
       </c>
-      <c r="I159" t="s">
+      <c r="I159" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J159" t="s">
@@ -8100,7 +8110,7 @@
       <c r="C160" t="s">
         <v>16</v>
       </c>
-      <c r="D160" s="3">
+      <c r="D160" s="2">
         <v>1</v>
       </c>
       <c r="E160">
@@ -8115,7 +8125,7 @@
       <c r="H160">
         <v>95</v>
       </c>
-      <c r="I160" t="s">
+      <c r="I160" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J160" t="s">
@@ -8147,7 +8157,7 @@
       <c r="C161" t="s">
         <v>16</v>
       </c>
-      <c r="D161" s="3">
+      <c r="D161" s="2">
         <v>2</v>
       </c>
       <c r="E161">
@@ -8162,7 +8172,7 @@
       <c r="H161">
         <v>96</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I161" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J161" t="s">
@@ -8194,7 +8204,7 @@
       <c r="C162" t="s">
         <v>16</v>
       </c>
-      <c r="D162" s="3">
+      <c r="D162" s="2">
         <v>1</v>
       </c>
       <c r="E162">
@@ -8209,7 +8219,7 @@
       <c r="H162">
         <v>97</v>
       </c>
-      <c r="I162" t="s">
+      <c r="I162" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J162" t="s">
@@ -8241,7 +8251,7 @@
       <c r="C163" t="s">
         <v>16</v>
       </c>
-      <c r="D163" s="3">
+      <c r="D163" s="2">
         <v>4</v>
       </c>
       <c r="E163">
@@ -8256,7 +8266,7 @@
       <c r="H163">
         <v>98</v>
       </c>
-      <c r="I163" t="s">
+      <c r="I163" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J163" t="s">
@@ -8288,7 +8298,7 @@
       <c r="C164" t="s">
         <v>16</v>
       </c>
-      <c r="D164" s="3">
+      <c r="D164" s="2">
         <v>2</v>
       </c>
       <c r="E164">
@@ -8303,7 +8313,7 @@
       <c r="H164">
         <v>99</v>
       </c>
-      <c r="I164" t="s">
+      <c r="I164" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J164" t="s">
@@ -8335,7 +8345,7 @@
       <c r="C165" t="s">
         <v>16</v>
       </c>
-      <c r="D165" s="3">
+      <c r="D165" s="2">
         <v>1</v>
       </c>
       <c r="E165">
@@ -8350,7 +8360,7 @@
       <c r="H165">
         <v>100</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I165" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J165" t="s">
@@ -8382,7 +8392,7 @@
       <c r="C166" t="s">
         <v>16</v>
       </c>
-      <c r="D166" s="3">
+      <c r="D166" s="2">
         <v>4</v>
       </c>
       <c r="E166">
@@ -8397,7 +8407,7 @@
       <c r="H166">
         <v>101</v>
       </c>
-      <c r="I166" t="s">
+      <c r="I166" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J166" t="s">
@@ -8429,7 +8439,7 @@
       <c r="C167" t="s">
         <v>16</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D167" s="2">
         <v>3</v>
       </c>
       <c r="E167">
@@ -8444,7 +8454,7 @@
       <c r="H167">
         <v>102</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I167" s="13" t="s">
         <v>23</v>
       </c>
       <c r="J167" t="s">
@@ -8476,7 +8486,7 @@
       <c r="C168" t="s">
         <v>16</v>
       </c>
-      <c r="D168" s="3">
+      <c r="D168" s="2">
         <v>3</v>
       </c>
       <c r="E168">
@@ -8491,7 +8501,7 @@
       <c r="H168">
         <v>103</v>
       </c>
-      <c r="I168" t="s">
+      <c r="I168" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J168" t="s">
@@ -8523,7 +8533,7 @@
       <c r="C169" t="s">
         <v>16</v>
       </c>
-      <c r="D169" s="3">
+      <c r="D169" s="2">
         <v>3</v>
       </c>
       <c r="E169">
@@ -8538,7 +8548,7 @@
       <c r="H169">
         <v>104</v>
       </c>
-      <c r="I169" t="s">
+      <c r="I169" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J169" t="s">
@@ -8570,7 +8580,7 @@
       <c r="C170" t="s">
         <v>16</v>
       </c>
-      <c r="D170" s="3">
+      <c r="D170" s="2">
         <v>4</v>
       </c>
       <c r="E170">
@@ -8585,7 +8595,7 @@
       <c r="H170">
         <v>105</v>
       </c>
-      <c r="I170" t="s">
+      <c r="I170" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J170" t="s">
@@ -8617,7 +8627,7 @@
       <c r="C171" t="s">
         <v>16</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D171" s="2">
         <v>4</v>
       </c>
       <c r="E171">
@@ -8632,7 +8642,7 @@
       <c r="H171">
         <v>106</v>
       </c>
-      <c r="I171" s="1" t="s">
+      <c r="I171" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J171" t="s">
@@ -8664,7 +8674,7 @@
       <c r="C172" t="s">
         <v>16</v>
       </c>
-      <c r="D172" s="3">
+      <c r="D172" s="2">
         <v>1</v>
       </c>
       <c r="E172">
@@ -8679,7 +8689,7 @@
       <c r="H172">
         <v>107</v>
       </c>
-      <c r="I172" t="s">
+      <c r="I172" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J172" t="s">
@@ -8711,7 +8721,7 @@
       <c r="C173" t="s">
         <v>16</v>
       </c>
-      <c r="D173" s="3">
+      <c r="D173" s="2">
         <v>1</v>
       </c>
       <c r="E173">
@@ -8726,7 +8736,7 @@
       <c r="H173">
         <v>108</v>
       </c>
-      <c r="I173" t="s">
+      <c r="I173" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J173" t="s">
@@ -8758,7 +8768,7 @@
       <c r="C174" t="s">
         <v>16</v>
       </c>
-      <c r="D174" s="3">
+      <c r="D174" s="2">
         <v>4</v>
       </c>
       <c r="E174">
@@ -8773,7 +8783,7 @@
       <c r="H174">
         <v>109</v>
       </c>
-      <c r="I174" t="s">
+      <c r="I174" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J174" t="s">
@@ -8805,7 +8815,7 @@
       <c r="C175" t="s">
         <v>16</v>
       </c>
-      <c r="D175" s="3">
+      <c r="D175" s="2">
         <v>1</v>
       </c>
       <c r="E175">
@@ -8820,7 +8830,7 @@
       <c r="H175">
         <v>110</v>
       </c>
-      <c r="I175" t="s">
+      <c r="I175" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J175" t="s">
@@ -8852,7 +8862,7 @@
       <c r="C176" t="s">
         <v>16</v>
       </c>
-      <c r="D176" s="3">
+      <c r="D176" s="2">
         <v>1</v>
       </c>
       <c r="E176">
@@ -8867,7 +8877,7 @@
       <c r="H176">
         <v>111</v>
       </c>
-      <c r="I176" t="s">
+      <c r="I176" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J176" t="s">
@@ -8899,7 +8909,7 @@
       <c r="C177" t="s">
         <v>16</v>
       </c>
-      <c r="D177" s="3">
+      <c r="D177" s="2">
         <v>1</v>
       </c>
       <c r="E177">
@@ -8914,7 +8924,7 @@
       <c r="H177">
         <v>112</v>
       </c>
-      <c r="I177" t="s">
+      <c r="I177" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J177" t="s">
@@ -8946,7 +8956,7 @@
       <c r="C178" t="s">
         <v>16</v>
       </c>
-      <c r="D178" s="3">
+      <c r="D178" s="2">
         <v>4</v>
       </c>
       <c r="E178">
@@ -8961,7 +8971,7 @@
       <c r="H178">
         <v>113</v>
       </c>
-      <c r="I178" t="s">
+      <c r="I178" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J178" t="s">
@@ -8993,7 +9003,7 @@
       <c r="C179" t="s">
         <v>16</v>
       </c>
-      <c r="D179" s="3">
+      <c r="D179" s="2">
         <v>5</v>
       </c>
       <c r="E179">
@@ -9008,7 +9018,7 @@
       <c r="H179">
         <v>114</v>
       </c>
-      <c r="I179" t="s">
+      <c r="I179" s="13" t="s">
         <v>32</v>
       </c>
       <c r="J179" t="s">
@@ -9040,7 +9050,7 @@
       <c r="C180" t="s">
         <v>16</v>
       </c>
-      <c r="D180" s="3">
+      <c r="D180" s="2">
         <v>4</v>
       </c>
       <c r="E180">
@@ -9055,7 +9065,7 @@
       <c r="H180">
         <v>115</v>
       </c>
-      <c r="I180" s="1" t="s">
+      <c r="I180" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J180" t="s">
@@ -9087,7 +9097,7 @@
       <c r="C181" t="s">
         <v>16</v>
       </c>
-      <c r="D181" s="3">
+      <c r="D181" s="2">
         <v>5</v>
       </c>
       <c r="E181">
@@ -9102,7 +9112,7 @@
       <c r="H181">
         <v>116</v>
       </c>
-      <c r="I181" s="1" t="s">
+      <c r="I181" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J181" t="s">
@@ -9126,68 +9136,67 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G28:G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>50</v>
       </c>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>2</v>
+      <c r="A3" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
@@ -9197,16 +9206,19 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
@@ -9214,114 +9226,111 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="B11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>45</v>
+      <c r="A14" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>35</v>
+      <c r="A17" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>36</v>
+      <c r="A18" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>37</v>
+      <c r="A19" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>38</v>
+      <c r="A20" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
@@ -9331,28 +9340,45 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>